<commit_message>
Updae for full 2014 data
</commit_message>
<xml_diff>
--- a/Budget/sql.xlsx
+++ b/Budget/sql.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="31">
   <si>
     <t>cat</t>
   </si>
@@ -71,7 +71,7 @@
     <t>direct</t>
   </si>
   <si>
-    <t>facebook</t>
+    <t>display</t>
   </si>
   <si>
     <t>ios</t>
@@ -81,6 +81,21 @@
   </si>
   <si>
     <t>organic</t>
+  </si>
+  <si>
+    <t>Paid Facebook</t>
+  </si>
+  <si>
+    <t>referral</t>
+  </si>
+  <si>
+    <t>remarketing</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>youtube</t>
   </si>
   <si>
     <t>registrations</t>
@@ -192,22 +207,22 @@
         <v>1141.0</v>
       </c>
       <c r="C2" t="n">
-        <v>2087.0</v>
+        <v>2117.0</v>
       </c>
       <c r="D2" t="n">
-        <v>2590.0</v>
+        <v>2609.0</v>
       </c>
       <c r="E2" t="n">
-        <v>2641.0</v>
+        <v>2642.0</v>
       </c>
       <c r="F2" t="n">
-        <v>2238.0</v>
+        <v>2240.0</v>
       </c>
       <c r="G2" t="n">
-        <v>2453.0</v>
+        <v>2462.0</v>
       </c>
       <c r="H2" t="n">
-        <v>2582.0</v>
+        <v>2584.0</v>
       </c>
       <c r="I2" t="n">
         <v>2733.0</v>
@@ -225,7 +240,7 @@
         <v>3936.0</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -269,7 +284,7 @@
         <v>26.0</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
@@ -313,7 +328,7 @@
         <v>1381.0</v>
       </c>
       <c r="N4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
@@ -357,7 +372,7 @@
         <v>1733.0</v>
       </c>
       <c r="N5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
@@ -365,43 +380,43 @@
         <v>18</v>
       </c>
       <c r="B6" t="n">
-        <v>320.0</v>
+        <v>157.0</v>
       </c>
       <c r="C6" t="n">
-        <v>305.0</v>
+        <v>163.0</v>
       </c>
       <c r="D6" t="n">
-        <v>310.0</v>
+        <v>160.0</v>
       </c>
       <c r="E6" t="n">
-        <v>245.0</v>
+        <v>137.0</v>
       </c>
       <c r="F6" t="n">
-        <v>371.0</v>
+        <v>247.0</v>
       </c>
       <c r="G6" t="n">
-        <v>520.0</v>
+        <v>395.0</v>
       </c>
       <c r="H6" t="n">
-        <v>397.0</v>
+        <v>285.0</v>
       </c>
       <c r="I6" t="n">
-        <v>313.0</v>
+        <v>202.0</v>
       </c>
       <c r="J6" t="n">
-        <v>827.0</v>
+        <v>715.0</v>
       </c>
       <c r="K6" t="n">
-        <v>716.0</v>
+        <v>633.0</v>
       </c>
       <c r="L6" t="n">
-        <v>1134.0</v>
+        <v>933.0</v>
       </c>
       <c r="M6" t="n">
-        <v>832.0</v>
+        <v>657.0</v>
       </c>
       <c r="N6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -409,43 +424,43 @@
         <v>19</v>
       </c>
       <c r="B7" t="n">
-        <v>41.0</v>
+        <v>0.0</v>
       </c>
       <c r="C7" t="n">
-        <v>36.0</v>
+        <v>5.0</v>
       </c>
       <c r="D7" t="n">
-        <v>138.0</v>
+        <v>24.0</v>
       </c>
       <c r="E7" t="n">
-        <v>65.0</v>
+        <v>6.0</v>
       </c>
       <c r="F7" t="n">
-        <v>26.0</v>
+        <v>0.0</v>
       </c>
       <c r="G7" t="n">
-        <v>138.0</v>
+        <v>0.0</v>
       </c>
       <c r="H7" t="n">
-        <v>56.0</v>
+        <v>0.0</v>
       </c>
       <c r="I7" t="n">
-        <v>24.0</v>
+        <v>0.0</v>
       </c>
       <c r="J7" t="n">
-        <v>165.0</v>
+        <v>9.0</v>
       </c>
       <c r="K7" t="n">
-        <v>72.0</v>
+        <v>0.0</v>
       </c>
       <c r="L7" t="n">
-        <v>70.0</v>
+        <v>0.0</v>
       </c>
       <c r="M7" t="n">
-        <v>37.0</v>
+        <v>0.0</v>
       </c>
       <c r="N7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -489,7 +504,7 @@
         <v>757.0</v>
       </c>
       <c r="N8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -533,7 +548,7 @@
         <v>7.0</v>
       </c>
       <c r="N9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -544,749 +559,749 @@
         <v>509.0</v>
       </c>
       <c r="C10" t="n">
-        <v>549.0</v>
+        <v>514.0</v>
       </c>
       <c r="D10" t="n">
-        <v>641.0</v>
+        <v>594.0</v>
       </c>
       <c r="E10" t="n">
-        <v>539.0</v>
+        <v>519.0</v>
       </c>
       <c r="F10" t="n">
-        <v>782.0</v>
+        <v>771.0</v>
       </c>
       <c r="G10" t="n">
-        <v>1080.0</v>
+        <v>1023.0</v>
       </c>
       <c r="H10" t="n">
-        <v>757.0</v>
+        <v>715.0</v>
       </c>
       <c r="I10" t="n">
-        <v>652.0</v>
+        <v>649.0</v>
       </c>
       <c r="J10" t="n">
-        <v>1563.0</v>
+        <v>1514.0</v>
       </c>
       <c r="K10" t="n">
-        <v>1299.0</v>
+        <v>1267.0</v>
       </c>
       <c r="L10" t="n">
-        <v>1909.0</v>
+        <v>1879.0</v>
       </c>
       <c r="M10" t="n">
-        <v>1684.0</v>
+        <v>1667.0</v>
       </c>
       <c r="N10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B11" t="n">
-        <v>1012.0</v>
+        <v>16.0</v>
       </c>
       <c r="C11" t="n">
-        <v>1792.0</v>
+        <v>23.0</v>
       </c>
       <c r="D11" t="n">
-        <v>2257.0</v>
+        <v>103.0</v>
       </c>
       <c r="E11" t="n">
-        <v>2276.0</v>
+        <v>50.0</v>
       </c>
       <c r="F11" t="n">
-        <v>1894.0</v>
+        <v>13.0</v>
       </c>
       <c r="G11" t="n">
-        <v>2114.0</v>
+        <v>94.0</v>
       </c>
       <c r="H11" t="n">
-        <v>2265.0</v>
+        <v>45.0</v>
       </c>
       <c r="I11" t="n">
-        <v>2387.0</v>
+        <v>16.0</v>
       </c>
       <c r="J11" t="n">
-        <v>2956.0</v>
+        <v>123.0</v>
       </c>
       <c r="K11" t="n">
-        <v>2914.0</v>
+        <v>52.0</v>
       </c>
       <c r="L11" t="n">
-        <v>3132.0</v>
+        <v>16.0</v>
       </c>
       <c r="M11" t="n">
-        <v>3488.0</v>
+        <v>6.0</v>
       </c>
       <c r="N11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B12" t="n">
-        <v>34.0</v>
+        <v>163.0</v>
       </c>
       <c r="C12" t="n">
-        <v>28.0</v>
+        <v>142.0</v>
       </c>
       <c r="D12" t="n">
-        <v>20.0</v>
+        <v>150.0</v>
       </c>
       <c r="E12" t="n">
-        <v>18.0</v>
+        <v>108.0</v>
       </c>
       <c r="F12" t="n">
-        <v>19.0</v>
+        <v>124.0</v>
       </c>
       <c r="G12" t="n">
-        <v>38.0</v>
+        <v>123.0</v>
       </c>
       <c r="H12" t="n">
-        <v>33.0</v>
+        <v>111.0</v>
       </c>
       <c r="I12" t="n">
-        <v>8.0</v>
+        <v>111.0</v>
       </c>
       <c r="J12" t="n">
-        <v>19.0</v>
+        <v>110.0</v>
       </c>
       <c r="K12" t="n">
-        <v>17.0</v>
+        <v>83.0</v>
       </c>
       <c r="L12" t="n">
-        <v>21.0</v>
+        <v>201.0</v>
       </c>
       <c r="M12" t="n">
-        <v>27.0</v>
+        <v>175.0</v>
       </c>
       <c r="N12" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B13" t="n">
         <v>0.0</v>
       </c>
       <c r="C13" t="n">
-        <v>142.0</v>
+        <v>0.0</v>
       </c>
       <c r="D13" t="n">
-        <v>247.0</v>
+        <v>4.0</v>
       </c>
       <c r="E13" t="n">
-        <v>253.0</v>
+        <v>13.0</v>
       </c>
       <c r="F13" t="n">
-        <v>197.0</v>
+        <v>9.0</v>
       </c>
       <c r="G13" t="n">
-        <v>341.0</v>
+        <v>48.0</v>
       </c>
       <c r="H13" t="n">
-        <v>203.0</v>
+        <v>40.0</v>
       </c>
       <c r="I13" t="n">
-        <v>251.0</v>
+        <v>3.0</v>
       </c>
       <c r="J13" t="n">
-        <v>792.0</v>
+        <v>40.0</v>
       </c>
       <c r="K13" t="n">
-        <v>625.0</v>
+        <v>31.0</v>
       </c>
       <c r="L13" t="n">
-        <v>837.0</v>
+        <v>29.0</v>
       </c>
       <c r="M13" t="n">
-        <v>671.0</v>
+        <v>17.0</v>
       </c>
       <c r="N13" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B14" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="M14" t="n">
         <v>31.0</v>
       </c>
-      <c r="C14" t="n">
-        <v>163.0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>234.0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>167.0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>309.0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>578.0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>317.0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>267.0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>1159.0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>1046.0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>1757.0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>1404.0</v>
-      </c>
       <c r="N14" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B15" t="n">
-        <v>283.0</v>
+        <v>0.0</v>
       </c>
       <c r="C15" t="n">
-        <v>268.0</v>
+        <v>0.0</v>
       </c>
       <c r="D15" t="n">
-        <v>275.0</v>
+        <v>0.0</v>
       </c>
       <c r="E15" t="n">
-        <v>222.0</v>
+        <v>0.0</v>
       </c>
       <c r="F15" t="n">
-        <v>338.0</v>
+        <v>0.0</v>
       </c>
       <c r="G15" t="n">
-        <v>452.0</v>
+        <v>2.0</v>
       </c>
       <c r="H15" t="n">
-        <v>357.0</v>
+        <v>1.0</v>
       </c>
       <c r="I15" t="n">
-        <v>287.0</v>
+        <v>0.0</v>
       </c>
       <c r="J15" t="n">
-        <v>712.0</v>
+        <v>2.0</v>
       </c>
       <c r="K15" t="n">
-        <v>621.0</v>
+        <v>0.0</v>
       </c>
       <c r="L15" t="n">
-        <v>978.0</v>
+        <v>0.0</v>
       </c>
       <c r="M15" t="n">
-        <v>679.0</v>
+        <v>0.0</v>
       </c>
       <c r="N15" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>28.0</v>
+        <v>1012.0</v>
       </c>
       <c r="C16" t="n">
-        <v>24.0</v>
+        <v>1821.0</v>
       </c>
       <c r="D16" t="n">
-        <v>80.0</v>
+        <v>2273.0</v>
       </c>
       <c r="E16" t="n">
-        <v>44.0</v>
+        <v>2277.0</v>
       </c>
       <c r="F16" t="n">
-        <v>21.0</v>
+        <v>1895.0</v>
       </c>
       <c r="G16" t="n">
-        <v>104.0</v>
+        <v>2121.0</v>
       </c>
       <c r="H16" t="n">
-        <v>39.0</v>
+        <v>2267.0</v>
       </c>
       <c r="I16" t="n">
-        <v>19.0</v>
+        <v>2387.0</v>
       </c>
       <c r="J16" t="n">
-        <v>108.0</v>
+        <v>2956.0</v>
       </c>
       <c r="K16" t="n">
-        <v>43.0</v>
+        <v>2914.0</v>
       </c>
       <c r="L16" t="n">
-        <v>50.0</v>
+        <v>3132.0</v>
       </c>
       <c r="M16" t="n">
-        <v>34.0</v>
+        <v>3488.0</v>
       </c>
       <c r="N16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0</v>
+        <v>34.0</v>
       </c>
       <c r="C17" t="n">
-        <v>24.0</v>
+        <v>28.0</v>
       </c>
       <c r="D17" t="n">
-        <v>196.0</v>
+        <v>20.0</v>
       </c>
       <c r="E17" t="n">
-        <v>143.0</v>
+        <v>18.0</v>
       </c>
       <c r="F17" t="n">
-        <v>127.0</v>
+        <v>19.0</v>
       </c>
       <c r="G17" t="n">
-        <v>209.0</v>
+        <v>38.0</v>
       </c>
       <c r="H17" t="n">
-        <v>159.0</v>
+        <v>33.0</v>
       </c>
       <c r="I17" t="n">
-        <v>145.0</v>
+        <v>8.0</v>
       </c>
       <c r="J17" t="n">
-        <v>519.0</v>
+        <v>19.0</v>
       </c>
       <c r="K17" t="n">
-        <v>421.0</v>
+        <v>17.0</v>
       </c>
       <c r="L17" t="n">
-        <v>493.0</v>
+        <v>21.0</v>
       </c>
       <c r="M17" t="n">
-        <v>391.0</v>
+        <v>27.0</v>
       </c>
       <c r="N17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B18" t="n">
         <v>0.0</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0</v>
+        <v>142.0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0</v>
+        <v>247.0</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0</v>
+        <v>253.0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0</v>
+        <v>197.0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0</v>
+        <v>341.0</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0</v>
+        <v>203.0</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0</v>
+        <v>251.0</v>
       </c>
       <c r="J18" t="n">
-        <v>3.0</v>
+        <v>792.0</v>
       </c>
       <c r="K18" t="n">
-        <v>14.0</v>
+        <v>625.0</v>
       </c>
       <c r="L18" t="n">
-        <v>18.0</v>
+        <v>837.0</v>
       </c>
       <c r="M18" t="n">
-        <v>6.0</v>
+        <v>671.0</v>
       </c>
       <c r="N18" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>460.0</v>
+        <v>31.0</v>
       </c>
       <c r="C19" t="n">
-        <v>489.0</v>
+        <v>163.0</v>
       </c>
       <c r="D19" t="n">
-        <v>554.0</v>
+        <v>234.0</v>
       </c>
       <c r="E19" t="n">
-        <v>474.0</v>
+        <v>167.0</v>
       </c>
       <c r="F19" t="n">
-        <v>700.0</v>
+        <v>309.0</v>
       </c>
       <c r="G19" t="n">
-        <v>926.0</v>
+        <v>578.0</v>
       </c>
       <c r="H19" t="n">
-        <v>665.0</v>
+        <v>317.0</v>
       </c>
       <c r="I19" t="n">
-        <v>577.0</v>
+        <v>267.0</v>
       </c>
       <c r="J19" t="n">
-        <v>1358.0</v>
+        <v>1159.0</v>
       </c>
       <c r="K19" t="n">
-        <v>1124.0</v>
+        <v>1046.0</v>
       </c>
       <c r="L19" t="n">
-        <v>1698.0</v>
+        <v>1757.0</v>
       </c>
       <c r="M19" t="n">
-        <v>1446.0</v>
+        <v>1404.0</v>
       </c>
       <c r="N19" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0</v>
+        <v>131.0</v>
       </c>
       <c r="C20" t="n">
-        <v>2287.0</v>
+        <v>137.0</v>
       </c>
       <c r="D20" t="n">
-        <v>3583.0</v>
+        <v>132.0</v>
       </c>
       <c r="E20" t="n">
-        <v>3638.0</v>
+        <v>116.0</v>
       </c>
       <c r="F20" t="n">
-        <v>3374.0</v>
+        <v>219.0</v>
       </c>
       <c r="G20" t="n">
-        <v>3671.0</v>
+        <v>340.0</v>
       </c>
       <c r="H20" t="n">
-        <v>3564.0</v>
+        <v>250.0</v>
       </c>
       <c r="I20" t="n">
-        <v>4013.0</v>
+        <v>181.0</v>
       </c>
       <c r="J20" t="n">
-        <v>4996.0</v>
+        <v>600.0</v>
       </c>
       <c r="K20" t="n">
-        <v>5029.0</v>
+        <v>537.0</v>
       </c>
       <c r="L20" t="n">
-        <v>5457.0</v>
+        <v>817.0</v>
       </c>
       <c r="M20" t="n">
-        <v>5843.0</v>
+        <v>558.0</v>
       </c>
       <c r="N20" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B21" t="n">
         <v>0.0</v>
       </c>
       <c r="C21" t="n">
-        <v>41.0</v>
+        <v>5.0</v>
       </c>
       <c r="D21" t="n">
-        <v>40.0</v>
+        <v>13.0</v>
       </c>
       <c r="E21" t="n">
-        <v>53.0</v>
+        <v>6.0</v>
       </c>
       <c r="F21" t="n">
-        <v>59.0</v>
+        <v>0.0</v>
       </c>
       <c r="G21" t="n">
-        <v>70.0</v>
+        <v>0.0</v>
       </c>
       <c r="H21" t="n">
-        <v>86.0</v>
+        <v>0.0</v>
       </c>
       <c r="I21" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="J21" t="n">
-        <v>61.0</v>
+        <v>8.0</v>
       </c>
       <c r="K21" t="n">
-        <v>53.0</v>
+        <v>0.0</v>
       </c>
       <c r="L21" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="M21" t="n">
-        <v>73.0</v>
+        <v>0.0</v>
       </c>
       <c r="N21" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B22" t="n">
         <v>0.0</v>
       </c>
       <c r="C22" t="n">
-        <v>300.0</v>
+        <v>24.0</v>
       </c>
       <c r="D22" t="n">
-        <v>1209.0</v>
+        <v>196.0</v>
       </c>
       <c r="E22" t="n">
-        <v>1568.0</v>
+        <v>143.0</v>
       </c>
       <c r="F22" t="n">
-        <v>2478.0</v>
+        <v>127.0</v>
       </c>
       <c r="G22" t="n">
-        <v>3187.0</v>
+        <v>209.0</v>
       </c>
       <c r="H22" t="n">
-        <v>3185.0</v>
+        <v>159.0</v>
       </c>
       <c r="I22" t="n">
-        <v>3200.0</v>
+        <v>145.0</v>
       </c>
       <c r="J22" t="n">
-        <v>6401.0</v>
+        <v>519.0</v>
       </c>
       <c r="K22" t="n">
-        <v>7208.0</v>
+        <v>421.0</v>
       </c>
       <c r="L22" t="n">
-        <v>9742.0</v>
+        <v>493.0</v>
       </c>
       <c r="M22" t="n">
-        <v>11202.0</v>
+        <v>391.0</v>
       </c>
       <c r="N22" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B23" t="n">
         <v>0.0</v>
       </c>
       <c r="C23" t="n">
-        <v>1878.0</v>
+        <v>0.0</v>
       </c>
       <c r="D23" t="n">
-        <v>2611.0</v>
+        <v>0.0</v>
       </c>
       <c r="E23" t="n">
-        <v>2155.0</v>
+        <v>0.0</v>
       </c>
       <c r="F23" t="n">
-        <v>3040.0</v>
+        <v>0.0</v>
       </c>
       <c r="G23" t="n">
-        <v>4141.0</v>
+        <v>0.0</v>
       </c>
       <c r="H23" t="n">
-        <v>2820.0</v>
+        <v>0.0</v>
       </c>
       <c r="I23" t="n">
-        <v>2831.0</v>
+        <v>0.0</v>
       </c>
       <c r="J23" t="n">
-        <v>5772.0</v>
+        <v>3.0</v>
       </c>
       <c r="K23" t="n">
-        <v>6447.0</v>
+        <v>14.0</v>
       </c>
       <c r="L23" t="n">
-        <v>8419.0</v>
+        <v>18.0</v>
       </c>
       <c r="M23" t="n">
-        <v>9464.0</v>
+        <v>6.0</v>
       </c>
       <c r="N23" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>24452.0</v>
+        <v>460.0</v>
       </c>
       <c r="C24" t="n">
-        <v>20837.0</v>
+        <v>455.0</v>
       </c>
       <c r="D24" t="n">
-        <v>21683.0</v>
+        <v>524.0</v>
       </c>
       <c r="E24" t="n">
-        <v>18204.0</v>
+        <v>457.0</v>
       </c>
       <c r="F24" t="n">
-        <v>25725.0</v>
+        <v>692.0</v>
       </c>
       <c r="G24" t="n">
-        <v>30472.0</v>
+        <v>882.0</v>
       </c>
       <c r="H24" t="n">
-        <v>20841.0</v>
+        <v>631.0</v>
       </c>
       <c r="I24" t="n">
-        <v>16971.0</v>
+        <v>574.0</v>
       </c>
       <c r="J24" t="n">
-        <v>33617.0</v>
+        <v>1319.0</v>
       </c>
       <c r="K24" t="n">
-        <v>36350.0</v>
+        <v>1101.0</v>
       </c>
       <c r="L24" t="n">
-        <v>43379.0</v>
+        <v>1674.0</v>
       </c>
       <c r="M24" t="n">
-        <v>42642.0</v>
+        <v>1433.0</v>
       </c>
       <c r="N24" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
       <c r="C25" t="n">
-        <v>30.0</v>
+        <v>14.0</v>
       </c>
       <c r="D25" t="n">
-        <v>79.0</v>
+        <v>56.0</v>
       </c>
       <c r="E25" t="n">
-        <v>48.0</v>
+        <v>32.0</v>
       </c>
       <c r="F25" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="K25" t="n">
         <v>29.0</v>
       </c>
-      <c r="G25" t="n">
-        <v>90.0</v>
-      </c>
-      <c r="H25" t="n">
-        <v>37.0</v>
-      </c>
-      <c r="I25" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="J25" t="n">
-        <v>90.0</v>
-      </c>
-      <c r="K25" t="n">
-        <v>40.0</v>
-      </c>
       <c r="L25" t="n">
-        <v>45.0</v>
+        <v>15.0</v>
       </c>
       <c r="M25" t="n">
-        <v>45.0</v>
+        <v>9.0</v>
       </c>
       <c r="N25" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.0</v>
+        <v>152.0</v>
       </c>
       <c r="C26" t="n">
-        <v>95.0</v>
+        <v>131.0</v>
       </c>
       <c r="D26" t="n">
-        <v>727.0</v>
+        <v>143.0</v>
       </c>
       <c r="E26" t="n">
-        <v>1099.0</v>
+        <v>106.0</v>
       </c>
       <c r="F26" t="n">
-        <v>1445.0</v>
+        <v>119.0</v>
       </c>
       <c r="G26" t="n">
-        <v>2007.0</v>
+        <v>112.0</v>
       </c>
       <c r="H26" t="n">
-        <v>1980.0</v>
+        <v>106.0</v>
       </c>
       <c r="I26" t="n">
-        <v>1870.0</v>
+        <v>106.0</v>
       </c>
       <c r="J26" t="n">
-        <v>3642.0</v>
+        <v>110.0</v>
       </c>
       <c r="K26" t="n">
-        <v>4461.0</v>
+        <v>84.0</v>
       </c>
       <c r="L26" t="n">
-        <v>5806.0</v>
+        <v>161.0</v>
       </c>
       <c r="M26" t="n">
-        <v>6919.0</v>
+        <v>121.0</v>
       </c>
       <c r="N26" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B27" t="n">
         <v>0.0</v>
@@ -1295,81 +1310,741 @@
         <v>0.0</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="G27" t="n">
-        <v>0.0</v>
+        <v>37.0</v>
       </c>
       <c r="H27" t="n">
-        <v>0.0</v>
+        <v>32.0</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="J27" t="n">
-        <v>202.0</v>
+        <v>31.0</v>
       </c>
       <c r="K27" t="n">
-        <v>269.0</v>
+        <v>22.0</v>
       </c>
       <c r="L27" t="n">
-        <v>361.0</v>
+        <v>23.0</v>
       </c>
       <c r="M27" t="n">
-        <v>406.0</v>
+        <v>13.0</v>
       </c>
       <c r="N27" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="N28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="K29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>2288.0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>3587.0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3638.0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>3375.0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3676.0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>3564.0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>4013.0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>4996.0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>5029.0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>5457.0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>5843.0</v>
+      </c>
+      <c r="N30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>86.0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="L31" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="M31" t="n">
+        <v>73.0</v>
+      </c>
+      <c r="N31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>300.0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1209.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1568.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2478.0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>3187.0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>3185.0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>3200.0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>6401.0</v>
+      </c>
+      <c r="K32" t="n">
+        <v>7208.0</v>
+      </c>
+      <c r="L32" t="n">
+        <v>9742.0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>11202.0</v>
+      </c>
+      <c r="N32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1878.0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2611.0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2155.0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>3040.0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>4141.0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>2820.0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>2831.0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>5772.0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>6447.0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>8419.0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>9464.0</v>
+      </c>
+      <c r="N33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>14843.0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>21244.0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>17905.0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>25246.0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>29945.0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>20497.0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>16712.0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>33276.0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>36074.0</v>
+      </c>
+      <c r="L34" t="n">
+        <v>42393.0</v>
+      </c>
+      <c r="M34" t="n">
+        <v>42102.0</v>
+      </c>
+      <c r="N34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>727.0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1099.0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1445.0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>2007.0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1980.0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1870.0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>3642.0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>4461.0</v>
+      </c>
+      <c r="L36" t="n">
+        <v>5806.0</v>
+      </c>
+      <c r="M36" t="n">
+        <v>6919.0</v>
+      </c>
+      <c r="N36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>202.0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>269.0</v>
+      </c>
+      <c r="L37" t="n">
+        <v>361.0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>406.0</v>
+      </c>
+      <c r="N37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
         <v>22</v>
       </c>
-      <c r="B28" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C28" t="n">
-        <v>2784.0</v>
-      </c>
-      <c r="D28" t="n">
-        <v>4259.0</v>
-      </c>
-      <c r="E28" t="n">
-        <v>3543.0</v>
-      </c>
-      <c r="F28" t="n">
-        <v>5183.0</v>
-      </c>
-      <c r="G28" t="n">
-        <v>6259.0</v>
-      </c>
-      <c r="H28" t="n">
-        <v>5046.0</v>
-      </c>
-      <c r="I28" t="n">
-        <v>4166.0</v>
-      </c>
-      <c r="J28" t="n">
-        <v>8360.0</v>
-      </c>
-      <c r="K28" t="n">
-        <v>7444.0</v>
-      </c>
-      <c r="L28" t="n">
-        <v>9587.0</v>
-      </c>
-      <c r="M28" t="n">
-        <v>9085.0</v>
-      </c>
-      <c r="N28" t="s">
+      <c r="B38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2773.0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>4222.0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3524.0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>5178.0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>6227.0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>5030.0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>4161.0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>8335.0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>7431.0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>9559.0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>9058.0</v>
+      </c>
+      <c r="N38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" t="n">
+        <v>24452.0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>5994.0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>438.0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>299.0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>478.0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>527.0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>344.0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>259.0</v>
+      </c>
+      <c r="J40" t="n">
+        <v>339.0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>275.0</v>
+      </c>
+      <c r="L40" t="n">
+        <v>986.0</v>
+      </c>
+      <c r="M40" t="n">
+        <v>540.0</v>
+      </c>
+      <c r="N40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
         <v>25</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="K41" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="L41" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="M41" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="N41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C42" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="K42" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="L42" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="M42" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="N42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J43" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N43" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>